<commit_message>
chore: update sample files to cover new features
</commit_message>
<xml_diff>
--- a/tests/sample_input_files/SOT_sample.xlsx
+++ b/tests/sample_input_files/SOT_sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_0BD228FA79F8C8CE8A160BFCABBB077F4A580918" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FCFFDE-02E8-4C31-B455-87F917AA295F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC608AEC-23D5-4CCC-B32E-804EDC2788B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -760,7 +760,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>